<commit_message>
added contact us page and video page
</commit_message>
<xml_diff>
--- a/6K185_DocShare_Ski/6k185 Project User Stories_with detials Updated1032013.xlsx
+++ b/6K185_DocShare_Ski/6k185 Project User Stories_with detials Updated1032013.xlsx
@@ -276,7 +276,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="135">
   <si>
     <t>Story ID</t>
   </si>
@@ -678,6 +678,9 @@
   </si>
   <si>
     <t>Assigned to Brayden</t>
+  </si>
+  <si>
+    <t>Assigned to Andrew - DONE (possible minor adjustments)</t>
   </si>
 </sst>
 </file>
@@ -1727,9 +1730,9 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="K41" sqref="K41"/>
+      <selection pane="bottomLeft" activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1742,7 +1745,7 @@
     <col min="8" max="8" width="29" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2313,7 +2316,7 @@
         <v>1</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added email to quiz
</commit_message>
<xml_diff>
--- a/6K185_DocShare_Ski/6k185 Project User Stories_with detials Updated1032013.xlsx
+++ b/6K185_DocShare_Ski/6k185 Project User Stories_with detials Updated1032013.xlsx
@@ -276,7 +276,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="135">
   <si>
     <t>Story ID</t>
   </si>
@@ -668,19 +668,7 @@
     <t>Redirected to previous page</t>
   </si>
   <si>
-    <t>Assigned to Andrew</t>
-  </si>
-  <si>
-    <t>Assigned to Yile</t>
-  </si>
-  <si>
     <t>Assigned to Wei</t>
-  </si>
-  <si>
-    <t>Assigned to Brayden</t>
-  </si>
-  <si>
-    <t>Assigned to Andrew - DONE (possible minor adjustments)</t>
   </si>
   <si>
     <t>Assigned to Wei
@@ -689,6 +677,12 @@
   <si>
     <t>Assigned to Wei
 Done except styling</t>
+  </si>
+  <si>
+    <t>Assigned to Andrew - DONE</t>
+  </si>
+  <si>
+    <t>Assigned to Yile &amp; Brayden</t>
   </si>
 </sst>
 </file>
@@ -1737,10 +1731,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1821,7 +1815,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2217,7 +2211,7 @@
         <v>1</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2324,7 +2318,7 @@
         <v>1</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -2351,7 +2345,7 @@
         <v>1</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2378,7 +2372,7 @@
         <v>1</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -2411,7 +2405,7 @@
         <v>1</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
@@ -2482,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished update committe information page
</commit_message>
<xml_diff>
--- a/6K185_DocShare_Ski/6k185 Project User Stories_with detials Updated1032013.xlsx
+++ b/6K185_DocShare_Ski/6k185 Project User Stories_with detials Updated1032013.xlsx
@@ -276,7 +276,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="134">
   <si>
     <t>Story ID</t>
   </si>
@@ -371,9 +371,6 @@
     <t>S202</t>
   </si>
   <si>
-    <t>S203</t>
-  </si>
-  <si>
     <t>Volunteer</t>
   </si>
   <si>
@@ -455,9 +452,6 @@
     <t>Create and edit volunteer information</t>
   </si>
   <si>
-    <t>Create and edit committee information text</t>
-  </si>
-  <si>
     <t>Receive an e-mail when a volunteer completes their quiz</t>
   </si>
   <si>
@@ -498,12 +492,6 @@
   </si>
   <si>
     <t>Create and Update Question Types</t>
-  </si>
-  <si>
-    <t>Create and Update Document Type</t>
-  </si>
-  <si>
-    <t>Create and edit document type</t>
   </si>
   <si>
     <t>Create and edit question type</t>
@@ -689,6 +677,9 @@
   </si>
   <si>
     <t>Create Update FAQ</t>
+  </si>
+  <si>
+    <t>Create and edit committee document</t>
   </si>
 </sst>
 </file>
@@ -1190,10 +1181,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1214,15 +1205,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>10</v>
@@ -1230,10 +1221,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1243,11 +1234,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,7 +1271,7 @@
     <row r="2" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1291,13 +1282,13 @@
         <v>28</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="E3" s="10">
         <v>2</v>
@@ -1308,13 +1299,13 @@
         <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="10">
         <v>1</v>
@@ -1325,13 +1316,13 @@
         <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="10">
         <v>1</v>
@@ -1342,13 +1333,13 @@
         <v>17</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="10">
         <v>1</v>
@@ -1359,13 +1350,13 @@
         <v>22</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="E7" s="6">
         <v>1</v>
@@ -1373,7 +1364,7 @@
     </row>
     <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1381,13 +1372,13 @@
         <v>29</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="10">
         <v>2</v>
@@ -1398,13 +1389,13 @@
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>59</v>
+        <v>133</v>
       </c>
       <c r="E11" s="10">
         <v>2</v>
@@ -1412,16 +1403,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>74</v>
+        <v>40</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>75</v>
+        <v>65</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="E12" s="10">
         <v>2</v>
@@ -1429,16 +1420,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E13" s="10">
         <v>2</v>
@@ -1446,16 +1437,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>73</v>
+        <v>52</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>76</v>
+        <v>65</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="E14" s="10">
         <v>2</v>
@@ -1465,14 +1456,14 @@
       <c r="A15" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>40</v>
+      <c r="B15" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="E15" s="10">
         <v>2</v>
@@ -1483,145 +1474,145 @@
         <v>54</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="10">
-        <v>2</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="C18" s="9"/>
     </row>
-    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>24</v>
+        <v>75</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>62</v>
+      <c r="D21" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="E21" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
-        <v>2</v>
+    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="E25" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E26" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>19</v>
+        <v>78</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="E27" s="6">
         <v>1</v>
@@ -1629,115 +1620,98 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" s="6">
-        <v>1</v>
+        <v>79</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="10">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="E29" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E30" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-    </row>
-    <row r="32" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="8"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-    </row>
-    <row r="37" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="8"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+    </row>
+    <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+    </row>
+    <row r="36" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
-      <c r="B40" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
-    </row>
-    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
-        <v>56</v>
+      <c r="B40" s="11"/>
+    </row>
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B41" s="6" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1785,25 +1759,25 @@
         <v>3</v>
       </c>
       <c r="E1" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="J1" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="K1" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1811,32 +1785,32 @@
         <v>13</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F2" s="21">
         <v>1</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H2" s="21"/>
       <c r="I2" s="21" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J2" s="21">
         <v>1</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1850,7 +1824,7 @@
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
@@ -1864,7 +1838,7 @@
       <c r="F4" s="21"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
@@ -1878,7 +1852,7 @@
       <c r="F5" s="21"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I5" s="21"/>
       <c r="J5" s="21"/>
@@ -1892,7 +1866,7 @@
       <c r="F6" s="21"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
@@ -1902,14 +1876,14 @@
       <c r="B7" s="21"/>
       <c r="C7" s="20"/>
       <c r="D7" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="21">
         <v>3</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="21"/>
@@ -1924,7 +1898,7 @@
       <c r="F8" s="21"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
@@ -1938,7 +1912,7 @@
       <c r="F9" s="21"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
@@ -1953,7 +1927,7 @@
         <v>4</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H10" s="15"/>
       <c r="I10" s="21"/>
@@ -1968,7 +1942,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
@@ -1983,7 +1957,7 @@
         <v>5</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="21"/>
@@ -1996,10 +1970,10 @@
       <c r="D13" s="15"/>
       <c r="E13" s="22"/>
       <c r="F13" s="21" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H13" s="15"/>
       <c r="I13" s="21"/>
@@ -2014,7 +1988,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I14" s="21"/>
       <c r="J14" s="21"/>
@@ -2028,7 +2002,7 @@
       <c r="F15" s="21"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I15" s="21"/>
       <c r="J15" s="21"/>
@@ -2042,7 +2016,7 @@
       <c r="F16" s="21"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I16" s="21"/>
       <c r="J16" s="21"/>
@@ -2056,7 +2030,7 @@
       <c r="F17" s="21"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I17" s="21"/>
       <c r="J17" s="21"/>
@@ -2068,10 +2042,10 @@
       <c r="D18" s="15"/>
       <c r="E18" s="22"/>
       <c r="F18" s="21" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="21"/>
@@ -2086,7 +2060,7 @@
       <c r="F19" s="21"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I19" s="21"/>
       <c r="J19" s="21"/>
@@ -2108,32 +2082,32 @@
         <v>14</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F21" s="21">
         <v>1</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H21" s="15"/>
       <c r="I21" s="21" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J21" s="21">
         <v>1</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2145,7 +2119,7 @@
       <c r="F22" s="21"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I22" s="21"/>
       <c r="J22" s="21"/>
@@ -2160,7 +2134,7 @@
         <v>2</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H23" s="15"/>
       <c r="I23" s="21"/>
@@ -2207,32 +2181,32 @@
         <v>17</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F27" s="21">
         <v>1</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H27" s="15"/>
       <c r="I27" s="21" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J27" s="21">
         <v>1</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2244,7 +2218,7 @@
       <c r="F28" s="21"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I28" s="21"/>
       <c r="J28" s="21"/>
@@ -2259,7 +2233,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H29" s="15"/>
       <c r="I29" s="21"/>
@@ -2274,7 +2248,7 @@
       <c r="F30" s="21"/>
       <c r="G30" s="15"/>
       <c r="H30" s="15" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I30" s="21"/>
       <c r="J30" s="21"/>
@@ -2320,53 +2294,53 @@
         <v>22</v>
       </c>
       <c r="B34" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>44</v>
       </c>
       <c r="E34" s="21"/>
       <c r="F34" s="21"/>
       <c r="G34" s="15"/>
       <c r="H34" s="21"/>
       <c r="I34" s="21" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J34" s="21">
         <v>1</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C35" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E35" s="21"/>
       <c r="F35" s="21"/>
       <c r="G35" s="15"/>
       <c r="H35" s="21"/>
       <c r="I35" s="21" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J35" s="21">
         <v>1</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2387,18 +2361,18 @@
       <c r="G36" s="15"/>
       <c r="H36" s="21"/>
       <c r="I36" s="21" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J36" s="21">
         <v>1</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B37" s="21" t="s">
         <v>18</v>
@@ -2410,23 +2384,23 @@
         <v>19</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F37" s="21">
         <v>1</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H37" s="21"/>
       <c r="I37" s="21" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J37" s="21">
         <v>1</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
@@ -2438,7 +2412,7 @@
       <c r="F38" s="21"/>
       <c r="G38" s="15"/>
       <c r="H38" s="21" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I38" s="21"/>
       <c r="J38" s="21"/>
@@ -2453,7 +2427,7 @@
         <v>2</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H39" s="21"/>
       <c r="I39" s="21"/>
@@ -2468,14 +2442,14 @@
       <c r="F40" s="21"/>
       <c r="G40" s="15"/>
       <c r="H40" s="21" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I40" s="21"/>
       <c r="J40" s="21"/>
     </row>
     <row r="41" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B41" s="22" t="s">
         <v>20</v>
@@ -2491,13 +2465,13 @@
       <c r="G41" s="15"/>
       <c r="H41" s="21"/>
       <c r="I41" s="21" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J41" s="21">
         <v>1</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
edit quiz page done wei
</commit_message>
<xml_diff>
--- a/6K185_DocShare_Ski/6k185 Project User Stories_with detials Updated1032013.xlsx
+++ b/6K185_DocShare_Ski/6k185 Project User Stories_with detials Updated1032013.xlsx
@@ -276,7 +276,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="137">
   <si>
     <t>Story ID</t>
   </si>
@@ -422,9 +422,6 @@
     <t>Create and Update Volunteer Information</t>
   </si>
   <si>
-    <t>Q:Are there are reports we want to run?</t>
-  </si>
-  <si>
     <t xml:space="preserve">System Admin </t>
   </si>
   <si>
@@ -443,9 +440,6 @@
     <t>S208</t>
   </si>
   <si>
-    <t>Quiz for interation 1, and Job description for Iteration 2 in case the database solution takes too much time.</t>
-  </si>
-  <si>
     <t>Watch and search for training videos for his/her committee</t>
   </si>
   <si>
@@ -554,9 +548,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Click on the 'Start Quiz' button</t>
-  </si>
-  <si>
     <t>System will display quiz Information for specific comiittee, the screen should display the following:</t>
   </si>
   <si>
@@ -566,15 +557,6 @@
     <t>`</t>
   </si>
   <si>
-    <t>1:Committee Title</t>
-  </si>
-  <si>
-    <t>2: Quiz Set</t>
-  </si>
-  <si>
-    <t>3: Submit Button</t>
-  </si>
-  <si>
     <t>the anwers will be selected:</t>
   </si>
   <si>
@@ -582,39 +564,6 @@
   </si>
   <si>
     <t>Click on the 'Submit Quiz' button</t>
-  </si>
-  <si>
-    <t>message box will pop up and verify quiz submmission</t>
-  </si>
-  <si>
-    <t>Verify whether I want to submit quiz</t>
-  </si>
-  <si>
-    <t>I can select yes and submit quiz</t>
-  </si>
-  <si>
-    <t>5a</t>
-  </si>
-  <si>
-    <t>The quiz will be submitted to the server</t>
-  </si>
-  <si>
-    <t>The correct answers will be displayed</t>
-  </si>
-  <si>
-    <t>message tells users they have finished the quiz successfully</t>
-  </si>
-  <si>
-    <t>system will send an email to the adminnistrator to verify the completion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5b </t>
-  </si>
-  <si>
-    <t>I can select no and go back to the quiz questions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I can continue editing answers </t>
   </si>
   <si>
     <t>Click on the Committtee Name</t>
@@ -680,6 +629,66 @@
   </si>
   <si>
     <t>Create and edit committee document</t>
+  </si>
+  <si>
+    <t>1: Quiz Set</t>
+  </si>
+  <si>
+    <t>2: Submit Button</t>
+  </si>
+  <si>
+    <t>Enter email address and click 'Submit' button</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>enter the correct email address</t>
+  </si>
+  <si>
+    <t>System will display the list of committees which users admit to and a Start quiz</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>enter a wrong email address</t>
+  </si>
+  <si>
+    <t>System will display a message showing 'Please Provide a valid e-mail address'</t>
+  </si>
+  <si>
+    <t>Select a committee and click on 'Start!' button</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>Click on 'Start!' button without select one committee</t>
+  </si>
+  <si>
+    <t>System will display a message showing 'Please select a committee to continue '</t>
+  </si>
+  <si>
+    <t>System checks to see if answers are all correct</t>
+  </si>
+  <si>
+    <t>4a</t>
+  </si>
+  <si>
+    <t>Answer all questions correctly</t>
+  </si>
+  <si>
+    <t>System redirect to comfirmation page and send a email to admin</t>
+  </si>
+  <si>
+    <t>4b</t>
+  </si>
+  <si>
+    <t>Did answer all questions correctly</t>
+  </si>
+  <si>
+    <t>System will display message to indicate which questions need to verify and stay on the quiz page</t>
   </si>
 </sst>
 </file>
@@ -790,7 +799,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -855,6 +864,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1181,10 +1193,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1208,12 +1220,12 @@
         <v>31</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>10</v>
@@ -1221,10 +1233,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1234,11 +1246,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,7 +1351,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E6" s="10">
         <v>1</v>
@@ -1364,7 +1376,7 @@
     </row>
     <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1375,10 +1387,10 @@
         <v>47</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E10" s="10">
         <v>2</v>
@@ -1392,10 +1404,10 @@
         <v>46</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="E11" s="10">
         <v>2</v>
@@ -1406,13 +1418,13 @@
         <v>40</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E12" s="10">
         <v>2</v>
@@ -1423,13 +1435,13 @@
         <v>44</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E13" s="10">
         <v>2</v>
@@ -1437,13 +1449,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>41</v>
@@ -1454,16 +1466,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>45</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E15" s="10">
         <v>2</v>
@@ -1471,16 +1483,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="E16" s="10"/>
     </row>
@@ -1496,7 +1508,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>23</v>
@@ -1505,7 +1517,7 @@
         <v>12</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E19" s="6">
         <v>2</v>
@@ -1513,7 +1525,7 @@
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>24</v>
@@ -1522,7 +1534,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E20" s="6">
         <v>2</v>
@@ -1530,7 +1542,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>26</v>
@@ -1552,16 +1564,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E24" s="6">
         <v>1</v>
@@ -1586,7 +1598,7 @@
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>18</v>
@@ -1603,7 +1615,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>20</v>
@@ -1620,16 +1632,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E28" s="10">
         <v>2</v>
@@ -1637,16 +1649,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E29" s="10">
         <v>3</v>
@@ -1657,21 +1669,21 @@
     </row>
     <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E32" s="6">
         <v>2</v>
@@ -1701,18 +1713,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
-      <c r="B39" s="6" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
-    </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B41" s="6" t="s">
-        <v>55</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1724,12 +1728,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,25 +1763,25 @@
         <v>3</v>
       </c>
       <c r="E1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="H1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="J1" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="K1" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1794,42 +1798,42 @@
         <v>38</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="F2" s="21">
         <v>1</v>
       </c>
-      <c r="G2" s="15" t="s">
-        <v>92</v>
+      <c r="G2" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="H2" s="21"/>
       <c r="I2" s="21" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="J2" s="21">
         <v>1</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="21"/>
       <c r="C3" s="20"/>
       <c r="D3" s="15"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="21">
-        <v>2</v>
-      </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15" t="s">
-        <v>93</v>
-      </c>
+      <c r="F3" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3" s="21"/>
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
     </row>
-    <row r="4" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
       <c r="B4" s="21"/>
       <c r="C4" s="20"/>
@@ -1837,27 +1841,29 @@
       <c r="E4" s="22"/>
       <c r="F4" s="21"/>
       <c r="G4" s="15"/>
-      <c r="H4" s="15" t="s">
-        <v>96</v>
+      <c r="H4" s="21" t="s">
+        <v>122</v>
       </c>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
     </row>
-    <row r="5" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="21"/>
       <c r="C5" s="20"/>
       <c r="D5" s="15"/>
       <c r="E5" s="22"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15" t="s">
-        <v>97</v>
-      </c>
+      <c r="F5" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="H5" s="21"/>
       <c r="I5" s="21"/>
       <c r="J5" s="21"/>
     </row>
-    <row r="6" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="21"/>
       <c r="C6" s="20"/>
@@ -1865,31 +1871,29 @@
       <c r="E6" s="22"/>
       <c r="F6" s="21"/>
       <c r="G6" s="15"/>
-      <c r="H6" s="15" t="s">
-        <v>98</v>
+      <c r="H6" s="21" t="s">
+        <v>125</v>
       </c>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
     </row>
-    <row r="7" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="21"/>
       <c r="C7" s="20"/>
-      <c r="D7" s="15" t="s">
-        <v>95</v>
-      </c>
+      <c r="D7" s="15"/>
       <c r="E7" s="22"/>
       <c r="F7" s="21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="H7" s="15"/>
+        <v>126</v>
+      </c>
+      <c r="H7" s="21"/>
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
     </row>
-    <row r="8" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
       <c r="B8" s="21"/>
       <c r="C8" s="20"/>
@@ -1898,12 +1902,12 @@
       <c r="F8" s="21"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
     </row>
-    <row r="9" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="21"/>
       <c r="C9" s="20"/>
@@ -1912,38 +1916,38 @@
       <c r="F9" s="21"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
     </row>
-    <row r="10" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="21"/>
       <c r="C10" s="20"/>
       <c r="D10" s="15"/>
       <c r="E10" s="22"/>
-      <c r="F10" s="21">
-        <v>4</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="H10" s="15"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15" t="s">
+        <v>118</v>
+      </c>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
     </row>
-    <row r="11" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="21"/>
       <c r="C11" s="20"/>
       <c r="D11" s="15"/>
       <c r="E11" s="22"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15" t="s">
-        <v>102</v>
-      </c>
+      <c r="F11" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" s="15"/>
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
     </row>
@@ -1953,33 +1957,33 @@
       <c r="C12" s="20"/>
       <c r="D12" s="15"/>
       <c r="E12" s="22"/>
-      <c r="F12" s="21">
-        <v>5</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="H12" s="15"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15" t="s">
+        <v>129</v>
+      </c>
       <c r="I12" s="21"/>
       <c r="J12" s="21"/>
     </row>
-    <row r="13" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="21"/>
       <c r="C13" s="20"/>
-      <c r="D13" s="15"/>
+      <c r="D13" s="15" t="s">
+        <v>92</v>
+      </c>
       <c r="E13" s="22"/>
-      <c r="F13" s="21" t="s">
-        <v>105</v>
+      <c r="F13" s="21">
+        <v>3</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="H13" s="15"/>
       <c r="I13" s="21"/>
       <c r="J13" s="21"/>
     </row>
-    <row r="14" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="B14" s="21"/>
       <c r="C14" s="20"/>
@@ -1988,7 +1992,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="I14" s="21"/>
       <c r="J14" s="21"/>
@@ -2002,26 +2006,28 @@
       <c r="F15" s="21"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="I15" s="21"/>
       <c r="J15" s="21"/>
     </row>
-    <row r="16" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="21"/>
       <c r="C16" s="20"/>
       <c r="D16" s="15"/>
       <c r="E16" s="22"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15" t="s">
-        <v>108</v>
-      </c>
+      <c r="F16" s="21">
+        <v>4</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="15"/>
       <c r="I16" s="21"/>
       <c r="J16" s="21"/>
     </row>
-    <row r="17" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="21"/>
       <c r="C17" s="20"/>
@@ -2030,28 +2036,28 @@
       <c r="F17" s="21"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="I17" s="21"/>
       <c r="J17" s="21"/>
     </row>
-    <row r="18" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="21"/>
       <c r="C18" s="20"/>
       <c r="D18" s="15"/>
       <c r="E18" s="22"/>
-      <c r="F18" s="21" t="s">
-        <v>110</v>
+      <c r="F18" s="24" t="s">
+        <v>131</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="21"/>
       <c r="J18" s="21"/>
     </row>
-    <row r="19" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
       <c r="B19" s="21"/>
       <c r="C19" s="20"/>
@@ -2060,101 +2066,107 @@
       <c r="F19" s="21"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="I19" s="21"/>
       <c r="J19" s="21"/>
     </row>
-    <row r="20" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="21"/>
       <c r="C20" s="20"/>
       <c r="D20" s="15"/>
       <c r="E20" s="22"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="15"/>
+      <c r="F20" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>135</v>
+      </c>
       <c r="H20" s="15"/>
       <c r="I20" s="21"/>
       <c r="J20" s="21"/>
     </row>
     <row r="21" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+    </row>
+    <row r="22" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="20" t="s">
+      <c r="B22" s="21"/>
+      <c r="C22" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D22" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="F21" s="21">
+      <c r="E22" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="21">
         <v>1</v>
       </c>
-      <c r="G21" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="H21" s="15"/>
-      <c r="I21" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="J21" s="21">
+      <c r="G22" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="H22" s="15"/>
+      <c r="I22" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="J22" s="21">
         <v>1</v>
       </c>
-      <c r="K21" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-    </row>
-    <row r="23" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="K22" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
       <c r="B23" s="21"/>
       <c r="C23" s="20"/>
       <c r="D23" s="15"/>
       <c r="E23" s="22"/>
-      <c r="F23" s="21">
-        <v>2</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="H23" s="15"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15" t="s">
+        <v>97</v>
+      </c>
       <c r="I23" s="21"/>
       <c r="J23" s="21"/>
     </row>
-    <row r="24" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="20"/>
       <c r="B24" s="21"/>
       <c r="C24" s="20"/>
       <c r="D24" s="15"/>
       <c r="E24" s="22"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="15"/>
+      <c r="F24" s="21">
+        <v>2</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>98</v>
+      </c>
       <c r="H24" s="15"/>
       <c r="I24" s="21"/>
       <c r="J24" s="21"/>
     </row>
-    <row r="25" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
-      <c r="B25" s="21"/>
+      <c r="B25" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="C25" s="20"/>
       <c r="D25" s="15"/>
       <c r="E25" s="22"/>
@@ -2176,92 +2188,92 @@
       <c r="I26" s="21"/>
       <c r="J26" s="21"/>
     </row>
-    <row r="27" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+    <row r="27" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+    </row>
+    <row r="28" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="20" t="s">
+      <c r="B28" s="21"/>
+      <c r="C28" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="F27" s="21">
+      <c r="D28" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28" s="21">
         <v>1</v>
       </c>
-      <c r="G27" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="H27" s="15"/>
-      <c r="I27" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="J27" s="21">
+      <c r="G28" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H28" s="15"/>
+      <c r="I28" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="J28" s="21">
         <v>1</v>
       </c>
-      <c r="K27" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
+      <c r="K28" s="6" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="29" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="20"/>
       <c r="D29" s="16"/>
       <c r="E29" s="22"/>
-      <c r="F29" s="21">
-        <v>2</v>
-      </c>
-      <c r="G29" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="H29" s="15"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15" t="s">
+        <v>100</v>
+      </c>
       <c r="I29" s="21"/>
       <c r="J29" s="21"/>
     </row>
     <row r="30" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
+      <c r="B30" s="21"/>
       <c r="C30" s="20"/>
       <c r="D30" s="16"/>
       <c r="E30" s="22"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15" t="s">
-        <v>119</v>
-      </c>
+      <c r="F30" s="21">
+        <v>2</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="H30" s="15"/>
       <c r="I30" s="21"/>
       <c r="J30" s="21"/>
     </row>
-    <row r="31" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
+      <c r="B31" s="22" t="s">
+        <v>36</v>
+      </c>
       <c r="C31" s="20"/>
       <c r="D31" s="16"/>
       <c r="E31" s="22"/>
       <c r="F31" s="21"/>
       <c r="G31" s="15"/>
-      <c r="H31" s="21"/>
+      <c r="H31" s="15" t="s">
+        <v>102</v>
+      </c>
       <c r="I31" s="21"/>
       <c r="J31" s="21"/>
     </row>
@@ -2289,206 +2301,204 @@
       <c r="I33" s="21"/>
       <c r="J33" s="21"/>
     </row>
-    <row r="34" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="21"/>
+    <row r="34" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="22"/>
       <c r="F34" s="21"/>
       <c r="G34" s="15"/>
       <c r="H34" s="21"/>
-      <c r="I34" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="J34" s="21">
-        <v>1</v>
-      </c>
-      <c r="K34" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+    </row>
+    <row r="35" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="21" t="s">
-        <v>51</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B35" s="22"/>
       <c r="C35" s="21" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="E35" s="21"/>
       <c r="F35" s="21"/>
       <c r="G35" s="15"/>
       <c r="H35" s="21"/>
       <c r="I35" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J35" s="21">
         <v>1</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="22"/>
+      <c r="C36" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="E36" s="21"/>
       <c r="F36" s="21"/>
       <c r="G36" s="15"/>
       <c r="H36" s="21"/>
       <c r="I36" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J36" s="21">
         <v>1</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="22"/>
+      <c r="C37" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="F37" s="21">
-        <v>1</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>122</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="15"/>
       <c r="H37" s="21"/>
       <c r="I37" s="21" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="J37" s="21">
         <v>1</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-    </row>
-    <row r="39" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="F38" s="21">
+        <v>1</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="J38" s="21">
+        <v>1</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="21"/>
-      <c r="B39" s="21"/>
+      <c r="B39" s="21" t="s">
+        <v>50</v>
+      </c>
       <c r="C39" s="21"/>
       <c r="D39" s="15"/>
       <c r="E39" s="21"/>
-      <c r="F39" s="21">
-        <v>2</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="H39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="I39" s="21"/>
       <c r="J39" s="21"/>
     </row>
-    <row r="40" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
-      <c r="B40" s="21"/>
+      <c r="B40" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="C40" s="21"/>
       <c r="D40" s="15"/>
       <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="21" t="s">
-        <v>125</v>
-      </c>
+      <c r="F40" s="21">
+        <v>2</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="H40" s="21"/>
       <c r="I40" s="21"/>
       <c r="J40" s="21"/>
     </row>
-    <row r="41" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>21</v>
-      </c>
+    <row r="41" spans="1:11" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="21"/>
+      <c r="B41" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="21"/>
+      <c r="D41" s="15"/>
       <c r="E41" s="21"/>
       <c r="F41" s="21"/>
       <c r="G41" s="15"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="J41" s="21">
+      <c r="H41" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+    </row>
+    <row r="42" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="21"/>
+      <c r="C42" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="J42" s="21">
         <v>1</v>
       </c>
-      <c r="K41" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
+      <c r="K42" s="6" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="23"/>
       <c r="D43" s="23"/>
       <c r="E43" s="23"/>
@@ -2498,6 +2508,29 @@
       <c r="I43" s="23"/>
       <c r="J43" s="23"/>
     </row>
+    <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="23"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="23"/>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="23"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>